<commit_message>
Added Spikes to Backlog Health
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Quasar-Issues.xlsx
+++ b/blueprint-jira-better-excel/Quasar-Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{FF509376-6139-48DD-861A-2FE3772036A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{B063F739-C481-4F80-8DA7-A77B1AF03BD6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8715" tabRatio="688" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,18 +22,18 @@
     <sheet name="Progress Charts" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="issues">OFFSET(Issues!$A$1,0,0,COUNTA(Issues!$A$1:$A$9999),COUNTA(Issues!$A$1:$AAH$1)-1)</definedName>
+    <definedName name="issues">OFFSET(Issues!$A$1,0,0,COUNTA(Issues!$A$1:$A$9999),COUNTA(Issues!$A$1:$AAI$1)-1)</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId8"/>
+    <pivotCache cacheId="10" r:id="rId8"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="213">
   <si>
     <t>Status</t>
   </si>
@@ -423,9 +423,6 @@
   </si>
   <si>
     <t>&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>$[IF(OR(B2="Bug", B2="Epic"),"",IF(D2=V2, 0, N2))]&lt;/jt:forEach&gt;</t>
   </si>
   <si>
     <t>Component</t>
@@ -1068,6 +1065,30 @@
   </si>
   <si>
     <t>Story Decomposition Progress</t>
+  </si>
+  <si>
+    <t>Backlog Health</t>
+  </si>
+  <si>
+    <t>$[IF(OR(B2="Bug", B2="Epic"),"",IF(D2=V2, 0, N2))]</t>
+  </si>
+  <si>
+    <t>Rocket</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>$[IF(OR(E2="Story: Ready",E2="Tech Debt: Ready",AND(B2="Spike",E2="Story: New")), "Yes", "No")]&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>SPs</t>
   </si>
 </sst>
 </file>
@@ -6830,11 +6851,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43327.352745138887" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43334.333140509261" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
-  <cacheFields count="40">
+  <cacheFields count="41">
     <cacheField name="Key" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -6999,11 +7020,12 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Release" numFmtId="0">
-      <sharedItems containsBlank="1" count="4">
+      <sharedItems containsBlank="1" count="5">
         <s v="${issue.fixVersions.name}"/>
         <m/>
         <s v="Pegasus"/>
         <s v="Quasar"/>
+        <s v="Rocket"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Priority" numFmtId="0">
@@ -7047,6 +7069,14 @@
     </cacheField>
     <cacheField name="Different Story Points" numFmtId="0">
       <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Backlog Health" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <s v="$[IF(OR(E2=&quot;Story: Ready&quot;,E2=&quot;Tech Debt: Ready&quot;,AND(B2=&quot;Spike&quot;,E2=&quot;Story: New&quot;)), &quot;Yes&quot;, &quot;No&quot;)]&lt;/jt:forEach&gt;"/>
+        <m/>
+        <s v="Yes"/>
+        <s v="No"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Component Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Epic Remaining Estimate')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
     <cacheField name="Component Decomposition Progress" numFmtId="0" formula=" IFERROR(SUM('Epic Decomposed')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
@@ -7099,7 +7129,8 @@
     <x v="0"/>
     <x v="0"/>
     <s v="$[IF(B2=&quot;Epic&quot;, IF(AND(IFERROR(VALUE(P2), 0)&gt;0, P2=W2), &quot;Yes&quot;, &quot;No&quot;), &quot;&quot;)]"/>
-    <s v="$[IF(OR(B2=&quot;Bug&quot;, B2=&quot;Epic&quot;),&quot;&quot;,IF(D2=V2, 0, N2))]&lt;/jt:forEach&gt;"/>
+    <s v="$[IF(OR(B2=&quot;Bug&quot;, B2=&quot;Epic&quot;),&quot;&quot;,IF(D2=V2, 0, N2))]"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="&lt;jt:forEach items=&quot;${issues.subList(0, 0)}&quot; var=&quot;issue&quot; where=&quot;${issue.key = ''}&quot;&gt;"/>
@@ -7139,6 +7170,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7178,6 +7210,7 @@
     <x v="2"/>
     <m/>
     <m/>
+    <x v="2"/>
   </r>
   <r>
     <s v="key"/>
@@ -7217,6 +7250,7 @@
     <x v="3"/>
     <m/>
     <m/>
+    <x v="3"/>
   </r>
   <r>
     <s v="key"/>
@@ -7249,13 +7283,14 @@
     <m/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="4"/>
     <m/>
     <m/>
     <x v="4"/>
     <x v="4"/>
     <m/>
     <m/>
+    <x v="2"/>
   </r>
   <r>
     <s v="key"/>
@@ -7295,6 +7330,7 @@
     <x v="5"/>
     <m/>
     <m/>
+    <x v="3"/>
   </r>
   <r>
     <s v="key"/>
@@ -7334,6 +7370,7 @@
     <x v="6"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7373,6 +7410,7 @@
     <x v="7"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7412,6 +7450,7 @@
     <x v="8"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7451,6 +7490,7 @@
     <x v="9"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7490,6 +7530,7 @@
     <x v="10"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7529,6 +7570,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7568,6 +7610,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7607,6 +7650,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7646,6 +7690,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7685,6 +7730,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7724,6 +7770,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7763,6 +7810,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7802,6 +7850,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7841,6 +7890,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7880,6 +7930,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7919,6 +7970,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7958,6 +8010,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -7997,6 +8050,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8036,6 +8090,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8075,6 +8130,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8114,6 +8170,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8153,6 +8210,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8192,6 +8250,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8231,6 +8290,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8270,6 +8330,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8309,6 +8370,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8348,6 +8410,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8387,6 +8450,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8426,6 +8490,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8465,6 +8530,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8504,6 +8570,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8543,6 +8610,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8582,6 +8650,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8621,6 +8690,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8660,6 +8730,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8699,6 +8770,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8738,6 +8810,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8777,6 +8850,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8816,6 +8890,7 @@
     <x v="1"/>
     <m/>
     <m/>
+    <x v="1"/>
   </r>
   <r>
     <s v="key"/>
@@ -8855,14 +8930,15 @@
     <x v="1"/>
     <m/>
     <s v="&lt;/jt:forEach&gt;"/>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A5:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+  <pivotFields count="41">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="8">
@@ -8955,11 +9031,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item x="3"/>
         <item h="1" x="1"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8984,6 +9061,7 @@
     <pivotField subtotalTop="0" showAll="0" sortType="ascending"/>
     <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -9029,9 +9107,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="D5:E17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+  <pivotFields count="41">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -9124,11 +9202,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item x="3"/>
         <item h="1" x="1"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -9150,6 +9229,7 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -9223,9 +9303,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A5:B17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+  <pivotFields count="41">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -9318,11 +9398,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item x="3"/>
         <item h="1" x="1"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -9344,6 +9425,7 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -9412,9 +9494,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="J5:L15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+  <pivotFields count="41">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -9507,11 +9589,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item x="3"/>
         <item h="1" x="1"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -9533,6 +9616,7 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -9594,9 +9678,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="G41:H43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+  <pivotFields count="41">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -9689,11 +9773,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item x="3"/>
         <item h="1" x="1"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -9718,6 +9803,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -9758,16 +9844,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A24:C27" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A24:E28" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="41">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
         <item h="1" x="0"/>
         <item h="1" x="6"/>
         <item h="1" x="2"/>
-        <item h="1" x="4"/>
+        <item x="4"/>
         <item x="3"/>
         <item x="5"/>
         <item h="1" x="1"/>
@@ -9776,57 +9862,7 @@
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="47">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item h="1" x="3"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="22"/>
-        <item h="1" x="15"/>
-        <item h="1" x="18"/>
-        <item h="1" x="16"/>
-        <item h="1" x="13"/>
-        <item h="1" x="17"/>
-        <item h="1" x="10"/>
-        <item h="1" x="19"/>
-        <item x="12"/>
-        <item h="1" x="20"/>
-        <item h="1" x="11"/>
-        <item h="1" x="14"/>
-        <item h="1" x="21"/>
-        <item h="1" x="35"/>
-        <item h="1" x="28"/>
-        <item h="1" x="31"/>
-        <item h="1" x="29"/>
-        <item h="1" x="26"/>
-        <item h="1" x="30"/>
-        <item h="1" x="23"/>
-        <item h="1" x="32"/>
-        <item x="25"/>
-        <item h="1" x="33"/>
-        <item h="1" x="24"/>
-        <item h="1" x="27"/>
-        <item h="1" x="34"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -9853,11 +9889,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item x="3"/>
         <item h="1" x="1"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -9882,6 +9919,15 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -9889,7 +9935,10 @@
   <rowFields count="1">
     <field x="33"/>
   </rowFields>
-  <rowItems count="1">
+  <rowItems count="2">
+    <i>
+      <x v="6"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -9898,17 +9947,24 @@
     <field x="1"/>
     <field x="-2"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="4">
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
     <i t="grand" i="1">
-      <x v="1"/>
+      <x/>
     </i>
   </colItems>
   <pageFields count="2">
     <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
+    <pageField fld="37" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
@@ -9927,9 +9983,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A41:B43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+  <pivotFields count="41">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -10022,11 +10078,12 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="2"/>
         <item x="3"/>
         <item h="1" x="1"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -10051,6 +10108,7 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -10091,9 +10149,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" missingCaption="0" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Component">
   <location ref="A5:C8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="40">
+  <pivotFields count="41">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisCol" subtotalTop="0" showAll="0">
       <items count="8">
@@ -10160,16 +10218,18 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
+      <items count="6">
         <item h="1" x="0"/>
         <item h="1" x="1"/>
         <item h="1" x="2"/>
         <item x="3"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -10199,9 +10259,9 @@
     <dataField name="Story Estimate_x000a_(incl. Tech Debt &amp; Spikes)" fld="14" baseField="10" baseItem="1"/>
     <dataField name="Decomposed _x000a_(Ready, In Dev, Closed)" fld="22" baseField="10" baseItem="1"/>
     <dataField name="Remaining Estimate_x000a_(Not Closed/ Not Decomposed)" fld="16" baseField="10" baseItem="1"/>
-    <dataField name="Epic Decomposition Progress" fld="39" baseField="10" baseItem="0" numFmtId="9"/>
-    <dataField name="Story Decomposition Progress" fld="38" subtotal="count" baseField="10" baseItem="0"/>
-    <dataField name="Development Progress" fld="37" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
+    <dataField name="Epic Decomposition Progress" fld="40" baseField="10" baseItem="0" numFmtId="9"/>
+    <dataField name="Story Decomposition Progress" fld="39" subtotal="count" baseField="10" baseItem="0"/>
+    <dataField name="Development Progress" fld="38" subtotal="count" baseField="10" baseItem="1" numFmtId="9"/>
   </dataFields>
   <formats count="5">
     <format dxfId="9">
@@ -10589,58 +10649,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -10653,7 +10715,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10665,17 +10727,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -10691,7 +10753,7 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
         <v>122</v>
@@ -10714,19 +10776,16 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-      <pivotSelection pane="bottomRight" activeRow="1" previousRow="1" click="1" r:id="rId2">
-        <pivotArea field="30" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
-      </pivotSelection>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.73046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -10742,18 +10801,18 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="22"/>
       <c r="D1" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
       <c r="J1" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
@@ -10761,22 +10820,22 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
@@ -10841,7 +10900,7 @@
         <v>45</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
@@ -10856,7 +10915,7 @@
         <v>60</v>
       </c>
       <c r="M8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
@@ -10871,7 +10930,7 @@
         <v>58</v>
       </c>
       <c r="M9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
@@ -10886,7 +10945,7 @@
         <v>56</v>
       </c>
       <c r="M10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
@@ -10901,7 +10960,7 @@
         <v>55</v>
       </c>
       <c r="M11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -10916,7 +10975,7 @@
         <v>59</v>
       </c>
       <c r="M12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
@@ -10931,7 +10990,7 @@
         <v>54</v>
       </c>
       <c r="M13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
@@ -10946,7 +11005,7 @@
         <v>61</v>
       </c>
       <c r="M14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
@@ -10985,7 +11044,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -10994,18 +11053,18 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
@@ -11015,48 +11074,68 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" t="s">
         <v>135</v>
-      </c>
-      <c r="C25" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>45</v>
       </c>
+      <c r="B26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="17" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="G37" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
@@ -11075,13 +11154,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>50</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H41" s="16" t="s">
         <v>50</v>
@@ -11144,7 +11223,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -11152,10 +11231,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -11173,7 +11252,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -11193,7 +11272,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:AL57"/>
+  <dimension ref="A1:AM57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -11238,10 +11317,11 @@
     <col min="35" max="35" width="18.86328125" style="5" customWidth="1"/>
     <col min="36" max="36" width="19.86328125" style="5" customWidth="1"/>
     <col min="37" max="37" width="18.796875" style="5" customWidth="1"/>
-    <col min="38" max="16384" width="9.1328125" style="3"/>
+    <col min="38" max="38" width="17.53125" style="5" customWidth="1"/>
+    <col min="39" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -11315,25 +11395,25 @@
         <v>21</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>43</v>
@@ -11348,16 +11428,19 @@
         <v>124</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AL1" s="3" t="s">
-        <v>197</v>
+      <c r="AL1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:38" s="5" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:39" s="5" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>69</v>
       </c>
@@ -11431,25 +11514,25 @@
         <v>42</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z2" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AB2" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AC2" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AD2" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE2" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>46</v>
@@ -11464,21 +11547,24 @@
         <v>125</v>
       </c>
       <c r="AJ2" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AK2" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="AL2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="AM2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
@@ -11496,7 +11582,7 @@
       </c>
       <c r="W4" s="4"/>
       <c r="AE4" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AH4" s="4" t="s">
         <v>58</v>
@@ -11505,8 +11591,11 @@
         <v>58</v>
       </c>
       <c r="AJ4" s="4"/>
+      <c r="AL4" s="5" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
@@ -11526,7 +11615,7 @@
       </c>
       <c r="W5" s="4"/>
       <c r="AE5" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AH5" s="4" t="s">
         <v>56</v>
@@ -11535,8 +11624,11 @@
         <v>56</v>
       </c>
       <c r="AJ5" s="4"/>
+      <c r="AL5" s="5" t="s">
+        <v>209</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -11556,6 +11648,9 @@
         <v>59</v>
       </c>
       <c r="W6" s="4"/>
+      <c r="AE6" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="AH6" s="4" t="s">
         <v>59</v>
       </c>
@@ -11563,8 +11658,11 @@
         <v>59</v>
       </c>
       <c r="AJ6" s="4"/>
+      <c r="AL6" s="5" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -11588,8 +11686,11 @@
         <v>54</v>
       </c>
       <c r="AJ7" s="4"/>
+      <c r="AL7" s="5" t="s">
+        <v>209</v>
+      </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>53</v>
       </c>
@@ -11614,7 +11715,7 @@
       </c>
       <c r="AJ8" s="4"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -11637,7 +11738,7 @@
       </c>
       <c r="AJ9" s="4"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>53</v>
       </c>
@@ -11660,7 +11761,7 @@
       </c>
       <c r="AJ10" s="4"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>53</v>
       </c>
@@ -11683,7 +11784,7 @@
       </c>
       <c r="AJ11" s="4"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>53</v>
       </c>
@@ -11706,7 +11807,7 @@
       </c>
       <c r="AJ12" s="4"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -11725,7 +11826,7 @@
       <c r="AI13" s="4"/>
       <c r="AJ13" s="4"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
@@ -11744,7 +11845,7 @@
       <c r="AI14" s="4"/>
       <c r="AJ14" s="4"/>
     </row>
-    <row r="15" spans="1:38" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:39" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
@@ -11763,7 +11864,7 @@
       <c r="AI15" s="4"/>
       <c r="AJ15" s="4"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>53</v>
       </c>
@@ -12105,7 +12206,7 @@
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
@@ -12115,7 +12216,7 @@
       <c r="J1" s="51"/>
       <c r="K1" s="51"/>
       <c r="L1" s="51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M1" s="51"/>
       <c r="N1" s="51"/>
@@ -12125,7 +12226,7 @@
       <c r="R1" s="51"/>
       <c r="S1" s="51"/>
       <c r="T1" s="51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U1" s="51"/>
       <c r="V1" s="51"/>
@@ -12137,91 +12238,91 @@
     </row>
     <row r="2" spans="1:28" s="32" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="49" t="s">
-        <v>160</v>
-      </c>
       <c r="D2" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>127</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I2" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="K2" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>133</v>
-      </c>
       <c r="M2" s="47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N2" s="34" t="s">
         <v>127</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="R2" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="S2" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="R2" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="T2" s="38" t="s">
-        <v>133</v>
-      </c>
       <c r="U2" s="47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="V2" s="34" t="s">
         <v>127</v>
       </c>
       <c r="W2" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X2" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Y2" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z2" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AA2" s="35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AB2" s="40"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -12309,7 +12410,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="44">
         <v>43194</v>
@@ -12398,7 +12499,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="44">
         <v>43208</v>
@@ -12487,7 +12588,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6" s="44">
         <v>43222</v>
@@ -12579,7 +12680,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="44">
         <v>43236</v>
@@ -12671,7 +12772,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="44">
         <v>43250</v>
@@ -12763,7 +12864,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="44">
         <v>43264</v>
@@ -12855,7 +12956,7 @@
     </row>
     <row r="10" spans="1:28" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10" s="44">
         <v>43278</v>
@@ -12947,7 +13048,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" s="44">
         <v>43292</v>
@@ -13039,7 +13140,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="44">
         <v>43299</v>
@@ -13131,7 +13232,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="44">
         <v>43313</v>
@@ -13223,7 +13324,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B14" s="44">
         <v>43327</v>
@@ -13327,7 +13428,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="44">
         <v>43341</v>
@@ -13347,7 +13448,7 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B16" s="44">
         <v>43355</v>
@@ -13367,7 +13468,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B17" s="46">
         <v>43369</v>

</xml_diff>

<commit_message>
Fixed an issue with Backlog Health, use Groovy script instead of a formula
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Quasar-Issues.xlsx
+++ b/blueprint-jira-better-excel/Quasar-Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{B063F739-C481-4F80-8DA7-A77B1AF03BD6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{FA99E832-3077-4903-A66A-B9A78FF4F122}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8715" tabRatio="688" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="212">
   <si>
     <t>Status</t>
   </si>
@@ -1079,16 +1079,13 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>$[IF(OR(E2="Story: Ready",E2="Tech Debt: Ready",AND(B2="Spike",E2="Story: New")), "Yes", "No")]&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
     <t>SPs</t>
+  </si>
+  <si>
+    <t>${bpHelper.isInBacklogHealth(issue)}&lt;/jt:forEach&gt;</t>
   </si>
 </sst>
 </file>
@@ -6851,7 +6848,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43334.333140509261" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43334.694266087965" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46" xr:uid="{00000000-000A-0000-FFFF-FFFF13000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -6969,7 +6966,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Story Points" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="5" maxValue="20"/>
     </cacheField>
     <cacheField name="Stories Estimate" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -7072,10 +7069,10 @@
     </cacheField>
     <cacheField name="Backlog Health" numFmtId="0">
       <sharedItems containsBlank="1" count="4">
-        <s v="$[IF(OR(E2=&quot;Story: Ready&quot;,E2=&quot;Tech Debt: Ready&quot;,AND(B2=&quot;Spike&quot;,E2=&quot;Story: New&quot;)), &quot;Yes&quot;, &quot;No&quot;)]&lt;/jt:forEach&gt;"/>
+        <s v="${bpHelper.isInBacklogHealth(issue)}&lt;/jt:forEach&gt;"/>
         <m/>
         <s v="Yes"/>
-        <s v="No"/>
+        <s v="&lt;/jt:forEach&gt;"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Component Progress" numFmtId="0" formula=" IFERROR(1 - SUM('Epic Remaining Estimate')/SUM('Epic Total Estimate'),1)" databaseField="0"/>
@@ -7226,7 +7223,7 @@
     <x v="1"/>
     <m/>
     <m/>
-    <m/>
+    <n v="5"/>
     <m/>
     <m/>
     <m/>
@@ -7250,7 +7247,7 @@
     <x v="3"/>
     <m/>
     <m/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="key"/>
@@ -7266,7 +7263,7 @@
     <x v="1"/>
     <m/>
     <m/>
-    <m/>
+    <n v="10"/>
     <m/>
     <m/>
     <m/>
@@ -7306,7 +7303,7 @@
     <x v="1"/>
     <m/>
     <m/>
-    <m/>
+    <n v="20"/>
     <m/>
     <m/>
     <m/>
@@ -7330,7 +7327,7 @@
     <x v="5"/>
     <m/>
     <m/>
-    <x v="3"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="key"/>
@@ -7370,7 +7367,7 @@
     <x v="6"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="key"/>
@@ -7410,7 +7407,7 @@
     <x v="7"/>
     <m/>
     <m/>
-    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="key"/>
@@ -8929,8 +8926,8 @@
     <x v="1"/>
     <x v="1"/>
     <m/>
-    <s v="&lt;/jt:forEach&gt;"/>
-    <x v="1"/>
+    <m/>
+    <x v="3"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -9107,6 +9104,671 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="J5:L15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="41">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="47">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item h="1" x="22"/>
+        <item h="1" x="15"/>
+        <item h="1" x="18"/>
+        <item h="1" x="16"/>
+        <item h="1" x="13"/>
+        <item h="1" x="17"/>
+        <item h="1" x="10"/>
+        <item h="1" x="19"/>
+        <item h="1" x="12"/>
+        <item h="1" x="20"/>
+        <item h="1" x="11"/>
+        <item h="1" x="14"/>
+        <item h="1" x="21"/>
+        <item h="1" x="35"/>
+        <item h="1" x="28"/>
+        <item h="1" x="31"/>
+        <item h="1" x="29"/>
+        <item h="1" x="26"/>
+        <item h="1" x="30"/>
+        <item h="1" x="23"/>
+        <item h="1" x="32"/>
+        <item h="1" x="25"/>
+        <item h="1" x="33"/>
+        <item h="1" x="24"/>
+        <item h="1" x="27"/>
+        <item h="1" x="34"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" sortType="ascending">
+      <items count="12">
+        <item h="1" x="0"/>
+        <item x="6"/>
+        <item h="1" x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item h="1" x="8"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <pageFields count="2">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="3" baseItem="4"/>
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="3" baseItem="4"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="G41:H43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="41">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="47">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item h="1" x="3"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item h="1" x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item h="1" x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item h="1" x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" sortType="ascending"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
+      <items count="12">
+        <item h="1" x="0"/>
+        <item x="6"/>
+        <item h="1" x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item h="1" x="8"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="34"/>
+  </rowFields>
+  <rowItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A24:G29" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="41">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
+      <items count="12">
+        <item h="1" x="0"/>
+        <item x="6"/>
+        <item x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="1"/>
+        <item x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="1"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="37" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
+    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A41:B43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="41">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
+      <items count="8">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="47">
+        <item h="1" x="0"/>
+        <item h="1" x="41"/>
+        <item h="1" x="39"/>
+        <item h="1" x="43"/>
+        <item h="1" x="45"/>
+        <item h="1" x="36"/>
+        <item h="1" x="42"/>
+        <item h="1" x="38"/>
+        <item h="1" x="37"/>
+        <item h="1" x="40"/>
+        <item h="1" x="44"/>
+        <item h="1" x="8"/>
+        <item h="1" x="3"/>
+        <item h="1" x="9"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" x="22"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item h="1" x="16"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="10"/>
+        <item x="19"/>
+        <item x="12"/>
+        <item x="20"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="21"/>
+        <item h="1" x="35"/>
+        <item x="28"/>
+        <item x="31"/>
+        <item h="1" x="29"/>
+        <item x="26"/>
+        <item x="30"/>
+        <item x="23"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="33"/>
+        <item x="24"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item h="1" x="1"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
+      <items count="12">
+        <item h="1" x="0"/>
+        <item x="6"/>
+        <item h="1" x="10"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="4"/>
+        <item h="1" x="8"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="33"/>
+  </rowFields>
+  <rowItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="30" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000003000000}" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="D5:E17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="41">
@@ -9302,7 +9964,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
   <location ref="A5:B17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="41">
@@ -9480,661 +10142,6 @@
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Estimate in Days" fld="12" baseField="3" baseItem="4"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="J5:L15" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="41">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="47">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item h="1" x="22"/>
-        <item h="1" x="15"/>
-        <item h="1" x="18"/>
-        <item h="1" x="16"/>
-        <item h="1" x="13"/>
-        <item h="1" x="17"/>
-        <item h="1" x="10"/>
-        <item h="1" x="19"/>
-        <item h="1" x="12"/>
-        <item h="1" x="20"/>
-        <item h="1" x="11"/>
-        <item h="1" x="14"/>
-        <item h="1" x="21"/>
-        <item h="1" x="35"/>
-        <item h="1" x="28"/>
-        <item h="1" x="31"/>
-        <item h="1" x="29"/>
-        <item h="1" x="26"/>
-        <item h="1" x="30"/>
-        <item h="1" x="23"/>
-        <item h="1" x="32"/>
-        <item h="1" x="25"/>
-        <item h="1" x="33"/>
-        <item h="1" x="24"/>
-        <item h="1" x="27"/>
-        <item h="1" x="34"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item h="1" x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" sortType="ascending">
-      <items count="12">
-        <item h="1" x="0"/>
-        <item x="6"/>
-        <item h="1" x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item h="1" x="8"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </colFields>
-  <pageFields count="2">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="3" baseItem="4"/>
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="3" baseItem="4"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000005000000}" name="PivotTable7" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="G41:H43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="41">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="47">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item h="1" x="3"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="22"/>
-        <item x="15"/>
-        <item x="18"/>
-        <item h="1" x="16"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="10"/>
-        <item x="19"/>
-        <item x="12"/>
-        <item x="20"/>
-        <item x="11"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item h="1" x="35"/>
-        <item x="28"/>
-        <item x="31"/>
-        <item h="1" x="29"/>
-        <item x="26"/>
-        <item x="30"/>
-        <item x="23"/>
-        <item x="32"/>
-        <item x="25"/>
-        <item x="33"/>
-        <item x="24"/>
-        <item x="27"/>
-        <item x="34"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item h="1" x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" sortType="ascending"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
-      <items count="12">
-        <item h="1" x="0"/>
-        <item x="6"/>
-        <item h="1" x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item h="1" x="8"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="34"/>
-  </rowFields>
-  <rowItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="2">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A24:E28" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="41">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
-      <items count="12">
-        <item h="1" x="0"/>
-        <item x="6"/>
-        <item x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="1"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="2">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="37" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Count" fld="13" subtotal="count" baseField="26" baseItem="0"/>
-    <dataField name="SPs" fld="13" baseField="26" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000004000000}" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A41:B43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="41">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisCol" subtotalTop="0" showAll="0">
-      <items count="8">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="47">
-        <item h="1" x="0"/>
-        <item h="1" x="41"/>
-        <item h="1" x="39"/>
-        <item h="1" x="43"/>
-        <item h="1" x="45"/>
-        <item h="1" x="36"/>
-        <item h="1" x="42"/>
-        <item h="1" x="38"/>
-        <item h="1" x="37"/>
-        <item h="1" x="40"/>
-        <item h="1" x="44"/>
-        <item h="1" x="8"/>
-        <item h="1" x="3"/>
-        <item h="1" x="9"/>
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="2"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="22"/>
-        <item x="15"/>
-        <item x="18"/>
-        <item h="1" x="16"/>
-        <item x="13"/>
-        <item x="17"/>
-        <item x="10"/>
-        <item x="19"/>
-        <item x="12"/>
-        <item x="20"/>
-        <item x="11"/>
-        <item x="14"/>
-        <item x="21"/>
-        <item h="1" x="35"/>
-        <item x="28"/>
-        <item x="31"/>
-        <item h="1" x="29"/>
-        <item x="26"/>
-        <item x="30"/>
-        <item x="23"/>
-        <item x="32"/>
-        <item x="25"/>
-        <item x="33"/>
-        <item x="24"/>
-        <item x="27"/>
-        <item x="34"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item h="1" x="1"/>
-        <item h="1" x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="ascending">
-      <items count="12">
-        <item h="1" x="0"/>
-        <item x="6"/>
-        <item h="1" x="10"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="4"/>
-        <item h="1" x="8"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="33"/>
-  </rowFields>
-  <rowItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="2">
-    <pageField fld="30" hier="-1"/>
-    <pageField fld="4" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Different Story Points" fld="36" baseField="26" baseItem="1"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -10776,18 +10783,18 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.19921875" bestFit="1" customWidth="1"/>
@@ -11033,7 +11040,7 @@
       </c>
       <c r="E16" s="20"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>51</v>
       </c>
@@ -11042,7 +11049,7 @@
       </c>
       <c r="E17" s="20"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="22" t="s">
         <v>147</v>
       </c>
@@ -11051,7 +11058,7 @@
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>171</v>
       </c>
@@ -11059,7 +11066,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>205</v>
       </c>
@@ -11067,50 +11074,102 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B24" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>71</v>
       </c>
       <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" t="s">
         <v>134</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C26" t="s">
-        <v>212</v>
+        <v>210</v>
+      </c>
+      <c r="D26" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" t="s">
+        <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="20">
+        <v>1</v>
+      </c>
+      <c r="E27" s="20">
+        <v>5</v>
+      </c>
+      <c r="F27" s="20">
+        <v>1</v>
+      </c>
+      <c r="G27" s="20">
+        <v>5</v>
+      </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+        <v>59</v>
+      </c>
+      <c r="B28" s="20">
+        <v>1</v>
+      </c>
+      <c r="C28" s="20">
+        <v>10</v>
+      </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
+      <c r="F28" s="20">
+        <v>1</v>
+      </c>
+      <c r="G28" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="20">
+        <v>1</v>
+      </c>
+      <c r="C29" s="20">
+        <v>10</v>
+      </c>
+      <c r="D29" s="20">
+        <v>1</v>
+      </c>
+      <c r="E29" s="20">
+        <v>5</v>
+      </c>
+      <c r="F29" s="20">
+        <v>2</v>
+      </c>
+      <c r="G29" s="20">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="22" t="s">
@@ -11440,7 +11499,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="5" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:39" s="5" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>69</v>
       </c>
@@ -11553,7 +11612,7 @@
         <v>206</v>
       </c>
       <c r="AL2" s="15" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AM2" s="5" t="s">
         <v>11</v>
@@ -11610,6 +11669,9 @@
       </c>
       <c r="G5" s="5"/>
       <c r="J5" s="5"/>
+      <c r="N5" s="5">
+        <v>5</v>
+      </c>
       <c r="V5" s="4" t="s">
         <v>56</v>
       </c>
@@ -11625,7 +11687,7 @@
       </c>
       <c r="AJ5" s="4"/>
       <c r="AL5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.45">
@@ -11644,6 +11706,9 @@
       <c r="E6" s="19" t="s">
         <v>97</v>
       </c>
+      <c r="N6" s="5">
+        <v>10</v>
+      </c>
       <c r="V6" s="4" t="s">
         <v>59</v>
       </c>
@@ -11675,6 +11740,9 @@
       <c r="E7" s="19" t="s">
         <v>98</v>
       </c>
+      <c r="N7" s="5">
+        <v>20</v>
+      </c>
       <c r="V7" s="4" t="s">
         <v>54</v>
       </c>
@@ -11687,7 +11755,7 @@
       </c>
       <c r="AJ7" s="4"/>
       <c r="AL7" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.45">
@@ -11714,6 +11782,9 @@
         <v>60</v>
       </c>
       <c r="AJ8" s="4"/>
+      <c r="AL8" s="5" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
@@ -11737,6 +11808,9 @@
         <v>61</v>
       </c>
       <c r="AJ9" s="4"/>
+      <c r="AL9" s="5" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
@@ -12000,7 +12074,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:38" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>53</v>
       </c>
@@ -12008,7 +12082,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:38" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>53</v>
       </c>
@@ -12016,7 +12090,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:38" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>53</v>
       </c>
@@ -12024,7 +12098,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:38" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
         <v>53</v>
       </c>
@@ -12032,7 +12106,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>53</v>
       </c>
@@ -12040,7 +12114,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
         <v>53</v>
       </c>
@@ -12048,7 +12122,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
         <v>53</v>
       </c>
@@ -12056,7 +12130,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
         <v>53</v>
       </c>
@@ -12064,7 +12138,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
         <v>53</v>
       </c>
@@ -12072,7 +12146,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
         <v>53</v>
       </c>
@@ -12080,7 +12154,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
         <v>53</v>
       </c>
@@ -12088,7 +12162,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
         <v>53</v>
       </c>
@@ -12096,7 +12170,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:38" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
         <v>53</v>
       </c>
@@ -12104,7 +12178,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:38" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
         <v>53</v>
       </c>
@@ -12112,18 +12186,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="AK47" s="5" t="s">
+      <c r="AL47" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.45">
       <c r="AH48" s="4"/>
     </row>
     <row r="49" spans="34:34" x14ac:dyDescent="0.45">

</xml_diff>